<commit_message>
Changed the time limit again from 2-28 to 2-21 for the p2-p3 / Changed the error handing [Unbound local error} to find the internal p1,p2 and p3 if there is no existing external p1-p2-p3 / Changed the '#Making a new dataframe of the higher highs and higher lows approaching P3 in chronological order' to use the function to make a / 	new empty dataframe with the colummns time and price.
</commit_message>
<xml_diff>
--- a/numerical data.xlsx
+++ b/numerical data.xlsx
@@ -2546,11 +2546,11 @@
   <dimension ref="A1:AL658"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="R49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z64" sqref="Z64"/>
+      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
changed the wrongly saved AUDUSD values for the one with the external p1-p2-p3 are invalid but the internal one did give a valid BOS, January 113, 2025 Asia session
</commit_message>
<xml_diff>
--- a/numerical data.xlsx
+++ b/numerical data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25800" windowHeight="17250"/>
+    <workbookView windowWidth="25800" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Main data" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,12 +548,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,25 +1370,25 @@
     <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2546,11 +2540,11 @@
   <dimension ref="A1:AL658"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2613,7 +2607,7 @@
       </c>
       <c r="K1" s="39">
         <f>IFERROR(AVERAGE(J5:J9973)," ")</f>
-        <v>0.0224537037037037</v>
+        <v>0.0218855218855219</v>
       </c>
       <c r="L1" s="38" t="s">
         <v>9</v>
@@ -2636,11 +2630,11 @@
       </c>
       <c r="S1" s="99">
         <f>AVERAGE(S5:S9971)</f>
-        <v>0.00496632996632997</v>
+        <v>0.00479797979797982</v>
       </c>
       <c r="T1" s="99">
         <f>AVERAGE(T5:T9971)</f>
-        <v>0.00646043771043772</v>
+        <v>0.00606060606060606</v>
       </c>
       <c r="U1" s="99">
         <f>AVERAGE(U5:U9971)</f>
@@ -2656,11 +2650,11 @@
       </c>
       <c r="Y1" s="121">
         <f>AVERAGE(Y5:Y9971)</f>
-        <v>1.6405390064481</v>
+        <v>1.62538749129658</v>
       </c>
       <c r="Z1" s="121">
         <f>AVERAGE(Z5:Z9971)</f>
-        <v>1.40137261728171</v>
+        <v>1.41965063555972</v>
       </c>
       <c r="AA1" s="121">
         <f>AVERAGE(AA5:AA9971)</f>
@@ -2671,11 +2665,11 @@
       </c>
       <c r="AD1" s="121">
         <f>AVERAGE(AD5:AD9971)</f>
-        <v>0.245595454545467</v>
+        <v>0.245588484848497</v>
       </c>
       <c r="AE1" s="121">
         <f>AVERAGE(AE5:AE9971)</f>
-        <v>0.288499999999992</v>
+        <v>0.288493636363628</v>
       </c>
       <c r="AF1" s="121">
         <f>AVERAGE(AF5:AF9971)</f>
@@ -2690,11 +2684,11 @@
       </c>
       <c r="AJ1" s="121">
         <f>AVERAGE(AJ5:AJ9971)</f>
-        <v>1.2633949267906</v>
+        <v>1.26603229412141</v>
       </c>
       <c r="AK1" s="121">
         <f>AVERAGE(AK5:AK9971)</f>
-        <v>1.15953578462112</v>
+        <v>1.16993271163776</v>
       </c>
       <c r="AL1" s="142">
         <f>AVERAGE(AL5:AL9971)</f>
@@ -2798,7 +2792,7 @@
       </c>
       <c r="AK2" s="121">
         <f>MIN(AK5:AK9972)</f>
-        <v>0.816901408450753</v>
+        <v>1.03030303030323</v>
       </c>
       <c r="AL2" s="142">
         <f>MIN(AL5:AL9972)</f>
@@ -2844,7 +2838,7 @@
       </c>
       <c r="T3" s="101">
         <f>MAX(T5:T9973)</f>
-        <v>0.0194444444444444</v>
+        <v>0.0145833333333333</v>
       </c>
       <c r="U3" s="101">
         <f>MAX(U5:U9973)</f>
@@ -7843,11 +7837,11 @@
       </c>
       <c r="S63" s="116">
         <f t="shared" ref="S63:S67" si="0">IF(F63-E63&lt;&gt;0,F63-E63,"")</f>
-        <v>0.00208333333333333</v>
+        <v>0.00208333333333399</v>
       </c>
       <c r="T63" s="116">
         <f t="shared" ref="T63:T67" si="1">IF(G63-F63&lt;&gt;0,G63-F63,"")</f>
-        <v>0.00138888888888888</v>
+        <v>0.00138888888888899</v>
       </c>
       <c r="U63" s="116">
         <f>IF(H63-G63&lt;&gt;0,H63-G63,"")</f>
@@ -7863,11 +7857,11 @@
       </c>
       <c r="Y63" s="136">
         <f>IFERROR(T63/S63,"")</f>
-        <v>0.666666666666667</v>
+        <v>0.666666666666507</v>
       </c>
       <c r="Z63" s="136">
         <f>IFERROR(U63/T63,"")</f>
-        <v>4</v>
+        <v>3.99999999999968</v>
       </c>
       <c r="AA63" s="136">
         <f>IFERROR(V63/U63,"")</f>
@@ -8010,11 +8004,11 @@
       </c>
       <c r="S65" s="104">
         <f t="shared" si="0"/>
-        <v>0.00277777777777777</v>
+        <v>0.00277777777777799</v>
       </c>
       <c r="T65" s="104">
         <f t="shared" si="1"/>
-        <v>0.00347222222222227</v>
+        <v>0.00347222222222204</v>
       </c>
       <c r="U65" s="104">
         <f>IF(H65-G65&lt;&gt;0,H65-G65,"")</f>
@@ -8030,11 +8024,11 @@
       </c>
       <c r="Y65" s="126">
         <f>IFERROR(T65/S65,"")</f>
-        <v>1.25000000000002</v>
+        <v>1.24999999999984</v>
       </c>
       <c r="Z65" s="126">
         <f>IFERROR(U65/T65,"")</f>
-        <v>2.19999999999996</v>
+        <v>2.2000000000001</v>
       </c>
       <c r="AA65" s="126">
         <f>IFERROR(V65/U65,"")</f>
@@ -8143,10 +8137,10 @@
         <v>23</v>
       </c>
       <c r="E67" s="30">
-        <v>0.143055555555556</v>
+        <v>0.161805555555556</v>
       </c>
       <c r="F67" s="30">
-        <v>0.152777777777778</v>
+        <v>0.165972222222222</v>
       </c>
       <c r="G67" s="30">
         <v>0.172222222222222</v>
@@ -8159,7 +8153,7 @@
       </c>
       <c r="J67" s="50">
         <f>I67-E67</f>
-        <v>0.04375</v>
+        <v>0.0250000000000004</v>
       </c>
       <c r="K67" s="51"/>
       <c r="L67" s="69">
@@ -8175,11 +8169,11 @@
       </c>
       <c r="S67" s="116">
         <f t="shared" si="0"/>
-        <v>0.00972222222222224</v>
+        <v>0.00416666666666665</v>
       </c>
       <c r="T67" s="116">
         <f t="shared" si="1"/>
-        <v>0.0194444444444444</v>
+        <v>0.00624999999999978</v>
       </c>
       <c r="U67" s="116">
         <f>IF(H67-G67&lt;&gt;0,H67-G67,"")</f>
@@ -8195,11 +8189,11 @@
       </c>
       <c r="Y67" s="136">
         <f>IFERROR(T67/S67,"")</f>
-        <v>1.99999999999999</v>
+        <v>1.49999999999995</v>
       </c>
       <c r="Z67" s="136">
         <f>IFERROR(U67/T67,"")</f>
-        <v>0.285714285714286</v>
+        <v>0.88888888888892</v>
       </c>
       <c r="AA67" s="136">
         <f>IFERROR(V67/U67,"")</f>
@@ -8225,10 +8219,10 @@
         <v>26</v>
       </c>
       <c r="E68" s="32">
-        <v>0.61626</v>
+        <v>0.61624</v>
       </c>
       <c r="F68" s="32">
-        <v>0.6156</v>
+        <v>0.61581</v>
       </c>
       <c r="G68" s="32">
         <v>0.61631</v>
@@ -8263,11 +8257,11 @@
       </c>
       <c r="AD68" s="140">
         <f t="shared" ref="AD68:AD130" si="4">IF(ABS($E68-$F68)&lt;&gt;0,ABS($E68-$F68),"")</f>
-        <v>0.000659999999999994</v>
+        <v>0.000430000000000041</v>
       </c>
       <c r="AE68" s="140">
         <f t="shared" ref="AE68:AE130" si="5">IF(ABS($F68-$G68)&lt;&gt;0,ABS($F68-$G68),"")</f>
-        <v>0.000709999999999988</v>
+        <v>0.000500000000000056</v>
       </c>
       <c r="AF68" s="140">
         <f t="shared" ref="AF68:AF130" si="6">IF(ABS($G68-$H68)&lt;&gt;0,ABS($G68-$H68),"")</f>
@@ -8283,11 +8277,11 @@
       </c>
       <c r="AJ68" s="161">
         <f t="shared" ref="AJ68" si="8">IFERROR(AE68/AD68,"")</f>
-        <v>1.07575757575757</v>
+        <v>1.16279069767444</v>
       </c>
       <c r="AK68" s="161">
         <f t="shared" ref="AK68" si="9">IFERROR(AF68/AE68,"")</f>
-        <v>0.816901408450753</v>
+        <v>1.15999999999992</v>
       </c>
       <c r="AL68" s="162">
         <f t="shared" ref="AL68" si="10">IFERROR(AG68/AF68,"")</f>

</xml_diff>